<commit_message>
Pcs Update Api Approve, Check,...
</commit_message>
<xml_diff>
--- a/Backend/PCS/PCS.LibraryMessage/PCS_Message.xlsx
+++ b/Backend/PCS/PCS.LibraryMessage/PCS_Message.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Enum</t>
   </si>
@@ -58,6 +58,36 @@
   </si>
   <si>
     <t>Dữ liệu đang được mở khóa</t>
+  </si>
+  <si>
+    <t>PcsProject__DuAnDaKetThuc</t>
+  </si>
+  <si>
+    <t>PcsPost__TrangThaiBaiDangKhongHopLe</t>
+  </si>
+  <si>
+    <t>PcsPost__TonTaiBaiDangKhongThuocDuAn</t>
+  </si>
+  <si>
+    <t>Dự án: {0} đã kết thúc</t>
+  </si>
+  <si>
+    <t>Trạng thái bài đăng không hợp lệ</t>
+  </si>
+  <si>
+    <t>Tồn tại bài đăng không thuộc dự án</t>
+  </si>
+  <si>
+    <t>PcsPost__DuAnChuaCoBaiDangNaoChuaDuyet</t>
+  </si>
+  <si>
+    <t>PcsPost__DuAnKhongCoBaiDangNaoHopLe</t>
+  </si>
+  <si>
+    <t>Dự án chưa có bài đăng nào chưa duyệt</t>
+  </si>
+  <si>
+    <t>Dự án không có bài đăng nào hợp lệ</t>
   </si>
 </sst>
 </file>
@@ -439,7 +469,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:B11"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -552,54 +582,83 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="2"/>
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>case Enum.: message = MessageViResource.; break;</v>
+        <v>case Enum.PcsProject__DuAnDaKetThuc: message = MessageViResource.PcsProject__DuAnDaKetThuc; break;</v>
       </c>
       <c r="F7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>case Enum.: message = MessageEnResource.; break;</v>
+        <v>case Enum.PcsProject__DuAnDaKetThuc: message = MessageEnResource.PcsProject__DuAnDaKetThuc; break;</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="E8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>case Enum.: message = MessageViResource.; break;</v>
+        <v>case Enum.PcsPost__TrangThaiBaiDangKhongHopLe: message = MessageViResource.PcsPost__TrangThaiBaiDangKhongHopLe; break;</v>
       </c>
       <c r="F8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>case Enum.: message = MessageEnResource.; break;</v>
+        <v>case Enum.PcsPost__TrangThaiBaiDangKhongHopLe: message = MessageEnResource.PcsPost__TrangThaiBaiDangKhongHopLe; break;</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>case Enum.: message = MessageViResource.; break;</v>
+        <v>case Enum.PcsPost__TonTaiBaiDangKhongThuocDuAn: message = MessageViResource.PcsPost__TonTaiBaiDangKhongThuocDuAn; break;</v>
       </c>
       <c r="F9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>case Enum.: message = MessageEnResource.; break;</v>
+        <v>case Enum.PcsPost__TonTaiBaiDangKhongThuocDuAn: message = MessageEnResource.PcsPost__TonTaiBaiDangKhongThuocDuAn; break;</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="E10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>case Enum.: message = MessageViResource.; break;</v>
+        <v>case Enum.PcsPost__DuAnChuaCoBaiDangNaoChuaDuyet: message = MessageViResource.PcsPost__DuAnChuaCoBaiDangNaoChuaDuyet; break;</v>
       </c>
       <c r="F10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>case Enum.: message = MessageEnResource.; break;</v>
+        <v>case Enum.PcsPost__DuAnChuaCoBaiDangNaoChuaDuyet: message = MessageEnResource.PcsPost__DuAnChuaCoBaiDangNaoChuaDuyet; break;</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>case Enum.: message = MessageViResource.; break;</v>
+        <v>case Enum.PcsPost__DuAnKhongCoBaiDangNaoHopLe: message = MessageViResource.PcsPost__DuAnKhongCoBaiDangNaoHopLe; break;</v>
       </c>
       <c r="F11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>case Enum.: message = MessageEnResource.; break;</v>
+        <v>case Enum.PcsPost__DuAnKhongCoBaiDangNaoHopLe: message = MessageEnResource.PcsPost__DuAnKhongCoBaiDangNaoHopLe; break;</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Pcs reject post and finish project
</commit_message>
<xml_diff>
--- a/Backend/PCS/PCS.LibraryMessage/PCS_Message.xlsx
+++ b/Backend/PCS/PCS.LibraryMessage/PCS_Message.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Enum</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>Dự án không có bài đăng nào hợp lệ</t>
+  </si>
+  <si>
+    <t>PcsEmployee__BanKhongCoQuyenThucHienChucNangNay</t>
+  </si>
+  <si>
+    <t>Bạn không có quyền thực hiện chức năng này</t>
+  </si>
+  <si>
+    <t>PcsPost__ThieuThongTinLyDoTuChoiDuyet</t>
+  </si>
+  <si>
+    <t>Thiếu thông tin lý do từ chối duyệt</t>
   </si>
 </sst>
 </file>
@@ -469,7 +481,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -662,23 +674,35 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>case Enum.: message = MessageViResource.; break;</v>
+        <v>case Enum.PcsEmployee__BanKhongCoQuyenThucHienChucNangNay: message = MessageViResource.PcsEmployee__BanKhongCoQuyenThucHienChucNangNay; break;</v>
       </c>
       <c r="F12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>case Enum.: message = MessageEnResource.; break;</v>
+        <v>case Enum.PcsEmployee__BanKhongCoQuyenThucHienChucNangNay: message = MessageEnResource.PcsEmployee__BanKhongCoQuyenThucHienChucNangNay; break;</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="E13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>case Enum.: message = MessageViResource.; break;</v>
+        <v>case Enum.PcsPost__ThieuThongTinLyDoTuChoiDuyet: message = MessageViResource.PcsPost__ThieuThongTinLyDoTuChoiDuyet; break;</v>
       </c>
       <c r="F13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>case Enum.: message = MessageEnResource.; break;</v>
+        <v>case Enum.PcsPost__ThieuThongTinLyDoTuChoiDuyet: message = MessageEnResource.PcsPost__ThieuThongTinLyDoTuChoiDuyet; break;</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Edit Approve, Reject, Finish
</commit_message>
<xml_diff>
--- a/Backend/PCS/PCS.LibraryMessage/PCS_Message.xlsx
+++ b/Backend/PCS/PCS.LibraryMessage/PCS_Message.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Enum</t>
   </si>
@@ -101,6 +101,24 @@
   <si>
     <t>Thiếu thông tin lý do từ chối duyệt</t>
   </si>
+  <si>
+    <t>PcsProject__TonTaiDuLieuDiaChi</t>
+  </si>
+  <si>
+    <t>PcsProject__TonTaiDuLieuBaiDang</t>
+  </si>
+  <si>
+    <t>Tồn tại dữ liệu địa chỉ</t>
+  </si>
+  <si>
+    <t>Tồn tại dữ liệu bài đăng</t>
+  </si>
+  <si>
+    <t>PcsPost__ChiDuocSuaXoaBaiDangKhiOTrangThai</t>
+  </si>
+  <si>
+    <t>Chỉ được sửa/xóa bài đăng khi đang ở tráng thái từ chối duyệt, chưa duyệt</t>
+  </si>
 </sst>
 </file>
 
@@ -159,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -173,6 +191,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,13 +502,13 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="74" style="3" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="58.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="6" style="3" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="2" customWidth="1"/>
@@ -706,33 +727,51 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="E14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>case Enum.: message = MessageViResource.; break;</v>
+        <v>case Enum.PcsProject__TonTaiDuLieuDiaChi: message = MessageViResource.PcsProject__TonTaiDuLieuDiaChi; break;</v>
       </c>
       <c r="F14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>case Enum.: message = MessageEnResource.; break;</v>
+        <v>case Enum.PcsProject__TonTaiDuLieuDiaChi: message = MessageEnResource.PcsProject__TonTaiDuLieuDiaChi; break;</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>case Enum.: message = MessageViResource.; break;</v>
+        <v>case Enum.PcsProject__TonTaiDuLieuBaiDang: message = MessageViResource.PcsProject__TonTaiDuLieuBaiDang; break;</v>
       </c>
       <c r="F15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>case Enum.: message = MessageEnResource.; break;</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>case Enum.PcsProject__TonTaiDuLieuBaiDang: message = MessageEnResource.PcsProject__TonTaiDuLieuBaiDang; break;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="E16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>case Enum.: message = MessageViResource.; break;</v>
+        <v>case Enum.PcsPost__ChiDuocSuaXoaBaiDangKhiOTrangThai: message = MessageViResource.PcsPost__ChiDuocSuaXoaBaiDangKhiOTrangThai; break;</v>
       </c>
       <c r="F16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>case Enum.: message = MessageEnResource.; break;</v>
+        <v>case Enum.PcsPost__ChiDuocSuaXoaBaiDangKhiOTrangThai: message = MessageEnResource.PcsPost__ChiDuocSuaXoaBaiDangKhiOTrangThai; break;</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.2">

</xml_diff>